<commit_message>
update wartung mit 10 tkm
</commit_message>
<xml_diff>
--- a/wartung_bmw.xlsx
+++ b/wartung_bmw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgi1sgm\phub\car_cost_comparisons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grzeg\hub\maxiumus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD8612-5973-4FE2-A79B-D0812723E309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B1596E-5F4E-48A2-B8CF-79090E8AD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WartungskostenBMW" sheetId="2" r:id="rId1"/>
@@ -104,7 +104,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -181,17 +181,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -207,17 +203,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -225,70 +215,64 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -341,6 +325,50 @@
         <a:xfrm>
           <a:off x="6870700" y="342900"/>
           <a:ext cx="5308873" cy="4864350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>520972</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CFA1B9E-E10C-D7C4-7B2A-EF60CE73CB46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12407900" y="393700"/>
+          <a:ext cx="5296172" cy="4661140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -689,10 +717,10 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6328125" bestFit="1" customWidth="1"/>
@@ -703,39 +731,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="29">
+      <c r="A2" s="23">
         <v>42093.636111111111</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="24">
         <v>76020</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="25">
         <v>399.99</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="30">
         <v>487.99</v>
       </c>
       <c r="F2" s="33">
@@ -743,35 +771,35 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="15">
+      <c r="A3" s="11">
         <v>42312.680555555547</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="19">
         <v>101599</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="20">
         <v>88</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="29">
+      <c r="A4" s="23">
         <v>42381.413194444453</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="24">
         <v>107211</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="25">
         <v>301.37</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="30">
         <v>1174.6799999999998</v>
       </c>
       <c r="F4" s="33">
@@ -779,67 +807,67 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>42487.329861111109</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="17">
         <v>118740</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="18">
         <v>80</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>42572</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="17">
         <v>127227</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="18">
         <v>253.41</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
+      <c r="A7" s="11">
         <v>42696</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="19">
         <v>138875</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="20">
         <v>539.9</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="29">
+      <c r="A8" s="23">
         <v>42818</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="24">
         <v>147744</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="25">
         <v>24.89</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="30">
         <v>393.89</v>
       </c>
       <c r="F8" s="33">
@@ -847,51 +875,51 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>42850.742361111108</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="17">
         <v>150551</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="18">
         <v>86.48</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
+      <c r="A10" s="11">
         <v>43021</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="19">
         <v>170748</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="20">
         <v>282.52</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="36">
+      <c r="A11" s="23">
         <v>43154.986111111109</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="24">
         <v>187098</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="25">
         <v>195.71</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="30">
         <v>642.03</v>
       </c>
       <c r="F11" s="33">
@@ -899,137 +927,137 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="34">
+      <c r="A12" s="1">
         <v>43238</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="17">
         <v>198569</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="18">
         <v>64.8</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="38">
+      <c r="A13" s="11">
         <v>43333.740972222222</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="19">
         <v>202187</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="20">
         <v>381.52</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="15">
+      <c r="A14" s="11">
         <v>43784</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="19">
         <v>222000</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="20">
         <v>24.89</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="15">
         <v>24.89</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="16">
         <v>2019</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>43879.716666666667</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="17">
         <v>229977</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="18">
         <v>611.47</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="32">
         <v>640.47</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="35">
         <v>2020</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
+      <c r="A16" s="11">
         <v>44169</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="19">
         <v>236900</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="20">
         <v>29</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="1">
         <v>44319</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="21">
         <v>241345</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="22">
         <v>29.75</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>29.75</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <v>2021</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="26">
         <f>($C$17-$C$2)/6.75</f>
         <v>24492.592592592591</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
         <f>SUM($D$2:$D$17)/6.75</f>
         <v>502.77037037037047</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="29">
         <f>$D$20/12</f>
         <v>41.897530864197542</v>
       </c>
@@ -1037,16 +1065,16 @@
     <row r="22" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F15:F16"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="E8:E10"/>
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F15:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1062,20 +1090,20 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1083,10 +1111,10 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>30000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>255</v>
       </c>
     </row>
@@ -1094,21 +1122,21 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>60000</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>325</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="16">
+      <c r="B5" s="12">
         <v>1</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="13">
         <v>90000</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="14">
         <v>425</v>
       </c>
     </row>
@@ -1116,10 +1144,10 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>40000</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>525</v>
       </c>
     </row>
@@ -1127,21 +1155,21 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>80000</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>685</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="16">
+      <c r="B8" s="12">
         <v>2</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>120000</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>935</v>
       </c>
     </row>
@@ -1149,10 +1177,10 @@
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>50000</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>895</v>
       </c>
     </row>
@@ -1160,10 +1188,10 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>100000</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>1145</v>
       </c>
     </row>
@@ -1171,10 +1199,10 @@
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>150000</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>1745</v>
       </c>
     </row>

</xml_diff>